<commit_message>
adding predictions from theory
</commit_message>
<xml_diff>
--- a/experiment/results/experiment_2/rating_matrix.xlsx
+++ b/experiment/results/experiment_2/rating_matrix.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="0" windowWidth="32340" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="5280" yWindow="0" windowWidth="30360" windowHeight="19980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rating_matrix.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -223,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,6 +248,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,7 +273,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -281,12 +289,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -294,6 +326,17 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -301,6 +344,17 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3353,4 +3407,2392 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="10.83203125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="10.83203125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L1" s="2">
+        <v>1</v>
+      </c>
+      <c r="M1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N1" s="2">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="2">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="2">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="2">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="2">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="2">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="2">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="2">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="2">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="2">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="2">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="2">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N33" s="2">
+        <v>0</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="2">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="2">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N36" s="2">
+        <v>0</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="2">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <v>1</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="2">
+        <v>0</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1</v>
+      </c>
+      <c r="J38" s="2">
+        <v>1</v>
+      </c>
+      <c r="K38" s="2">
+        <v>0</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
+        <v>1</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="2">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <v>1</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="2">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N40" s="2">
+        <v>0</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="2">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1</v>
+      </c>
+      <c r="J41" s="2">
+        <v>1</v>
+      </c>
+      <c r="K41" s="2">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
+        <v>1</v>
+      </c>
+      <c r="N41" s="2">
+        <v>0</v>
+      </c>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="2">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
+        <v>1</v>
+      </c>
+      <c r="N42" s="2">
+        <v>0</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1</v>
+      </c>
+      <c r="M43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N43" s="2">
+        <v>1</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="2">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N44" s="2">
+        <v>0</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" s="2">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1</v>
+      </c>
+      <c r="K45" s="2">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2">
+        <v>1</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L46" s="2">
+        <v>1</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N46" s="2">
+        <v>1</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="2">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1</v>
+      </c>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2">
+        <v>1</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+      <c r="M47" s="2">
+        <v>1</v>
+      </c>
+      <c r="N47" s="2">
+        <v>0</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" s="2">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1</v>
+      </c>
+      <c r="L48" s="2">
+        <v>0</v>
+      </c>
+      <c r="M48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N48" s="2">
+        <v>0</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" s="2">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0</v>
+      </c>
+      <c r="M49" s="2">
+        <v>1</v>
+      </c>
+      <c r="N49" s="2">
+        <v>0</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>